<commit_message>
updating paths to work on my machine
</commit_message>
<xml_diff>
--- a/projects/dfg_test_m0_office_blend.xlsx
+++ b/projects/dfg_test_m0_office_blend.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="2880" windowWidth="21210" windowHeight="2895" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="2880" windowWidth="21210" windowHeight="2895" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -1984,9 +1984,6 @@
     <t>OSM</t>
   </si>
   <si>
-    <t>nlong</t>
-  </si>
-  <si>
     <t>singlerun</t>
   </si>
   <si>
@@ -2647,12 +2644,6 @@
     <t>Elec EUI</t>
   </si>
   <si>
-    <t>../../cofee-measures/model0</t>
-  </si>
-  <si>
-    <t>../../cofee-measures/lib/</t>
-  </si>
-  <si>
     <t>Fraction of C</t>
   </si>
   <si>
@@ -2789,6 +2780,15 @@
   </si>
   <si>
     <t>Blend C</t>
+  </si>
+  <si>
+    <t>dgoldwas</t>
+  </si>
+  <si>
+    <t>../../../GitHub/cofee-measures/model0</t>
+  </si>
+  <si>
+    <t>../../../GitHub/cofee-measures/lib/</t>
   </si>
 </sst>
 </file>
@@ -7013,8 +7013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7050,7 +7050,7 @@
         <v>436</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>437</v>
@@ -7061,7 +7061,7 @@
         <v>456</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>647</v>
+        <v>913</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>457</v>
@@ -7072,7 +7072,7 @@
         <v>469</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>614</v>
@@ -7154,21 +7154,21 @@
         <v>39</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>911</v>
+        <v>908</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>868</v>
+        <v>914</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -7176,10 +7176,10 @@
         <v>26</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -7244,7 +7244,7 @@
         <v>451</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -7333,7 +7333,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>31</v>
@@ -7346,7 +7346,7 @@
         <v>29</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>878</v>
+        <v>875</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -7360,7 +7360,7 @@
         <v>38</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="E39" s="13" t="s">
         <v>449</v>
@@ -7374,10 +7374,10 @@
         <v>646</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -7388,7 +7388,7 @@
         <v>34</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="13" t="s">
@@ -7397,24 +7397,24 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>869</v>
+        <v>915</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="31" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>879</v>
+        <v>876</v>
       </c>
       <c r="C44" s="31" t="s">
-        <v>880</v>
+        <v>877</v>
       </c>
       <c r="D44" s="2"/>
     </row>
@@ -7444,9 +7444,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I26" sqref="I26"/>
+      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7544,7 +7544,7 @@
         <v>36</v>
       </c>
       <c r="F3" s="50" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="G3" s="15" t="s">
         <v>11</v>
@@ -7609,13 +7609,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>881</v>
+        <v>878</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>882</v>
+        <v>879</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>882</v>
+        <v>879</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>68</v>
@@ -7628,16 +7628,16 @@
         <v>21</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>883</v>
+        <v>880</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>884</v>
+        <v>881</v>
       </c>
       <c r="G5" s="31" t="s">
         <v>618</v>
       </c>
       <c r="I5" s="31" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="J5" s="31"/>
     </row>
@@ -7646,16 +7646,16 @@
         <v>21</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>885</v>
+        <v>882</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>886</v>
+        <v>883</v>
       </c>
       <c r="G6" s="31" t="s">
         <v>618</v>
       </c>
       <c r="I6" s="31" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="J6" s="31"/>
     </row>
@@ -7664,16 +7664,16 @@
         <v>21</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>887</v>
+        <v>884</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>888</v>
+        <v>885</v>
       </c>
       <c r="G7" s="31" t="s">
         <v>618</v>
       </c>
       <c r="I7" s="52" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
       <c r="J7" s="31"/>
     </row>
@@ -7682,16 +7682,16 @@
         <v>21</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
       <c r="G8" s="31" t="s">
         <v>618</v>
       </c>
       <c r="I8" s="52" t="s">
-        <v>892</v>
+        <v>889</v>
       </c>
       <c r="J8" s="31"/>
     </row>
@@ -7700,13 +7700,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>893</v>
+        <v>890</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
       <c r="E9" s="37" t="s">
         <v>233</v>
@@ -7719,13 +7719,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="37" t="s">
+        <v>654</v>
+      </c>
+      <c r="C10" s="37" t="s">
         <v>655</v>
       </c>
-      <c r="C10" s="37" t="s">
-        <v>656</v>
-      </c>
       <c r="D10" s="37" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="E10" s="37" t="s">
         <v>68</v>
@@ -7738,16 +7738,16 @@
         <v>21</v>
       </c>
       <c r="D11" s="30" t="s">
+        <v>661</v>
+      </c>
+      <c r="E11" s="30" t="s">
         <v>662</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>663</v>
       </c>
       <c r="G11" s="30" t="s">
         <v>104</v>
       </c>
       <c r="I11" s="30" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="12" spans="1:26" s="30" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
@@ -7755,16 +7755,16 @@
         <v>21</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="G12" s="30" t="s">
         <v>104</v>
       </c>
       <c r="I12" s="31" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
     </row>
     <row r="13" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -7772,13 +7772,13 @@
         <v>1</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="E13" s="37" t="s">
         <v>68</v>
@@ -7791,17 +7791,17 @@
         <v>21</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="F14" s="30"/>
       <c r="G14" s="31" t="s">
         <v>618</v>
       </c>
       <c r="I14" s="31" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -7817,13 +7817,13 @@
         <v>21</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="F15" s="31" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
       <c r="G15" s="31" t="s">
         <v>619</v>
@@ -7849,7 +7849,7 @@
       <c r="P15" s="4"/>
       <c r="Q15" s="3"/>
       <c r="R15" s="31" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
@@ -7857,10 +7857,10 @@
         <v>21</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="F16" s="30"/>
       <c r="G16" s="31" t="s">
@@ -7876,17 +7876,17 @@
         <v>21</v>
       </c>
       <c r="D17" s="31" t="s">
+        <v>807</v>
+      </c>
+      <c r="E17" s="31" t="s">
         <v>808</v>
-      </c>
-      <c r="E17" s="31" t="s">
-        <v>809</v>
       </c>
       <c r="F17" s="30"/>
       <c r="G17" s="30" t="s">
         <v>104</v>
       </c>
       <c r="I17" s="31" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="J17" s="31"/>
     </row>
@@ -7895,13 +7895,13 @@
         <v>1</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="E18" s="37" t="s">
         <v>68</v>
@@ -7914,17 +7914,17 @@
         <v>21</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="E19" s="31" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="F19" s="30"/>
       <c r="G19" s="31" t="s">
         <v>618</v>
       </c>
       <c r="I19" s="31" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -7940,13 +7940,13 @@
         <v>21</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>870</v>
+        <v>867</v>
       </c>
       <c r="E20" s="31" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="F20" s="31" t="s">
-        <v>875</v>
+        <v>872</v>
       </c>
       <c r="G20" s="31" t="s">
         <v>619</v>
@@ -7971,7 +7971,7 @@
       <c r="P20" s="4"/>
       <c r="Q20" s="3"/>
       <c r="R20" s="31" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -7979,10 +7979,10 @@
         <v>21</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E21" s="31" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="F21" s="30"/>
       <c r="G21" s="31" t="s">
@@ -7998,17 +7998,17 @@
         <v>21</v>
       </c>
       <c r="D22" s="31" t="s">
+        <v>807</v>
+      </c>
+      <c r="E22" s="31" t="s">
         <v>808</v>
-      </c>
-      <c r="E22" s="31" t="s">
-        <v>809</v>
       </c>
       <c r="F22" s="30"/>
       <c r="G22" s="30" t="s">
         <v>104</v>
       </c>
       <c r="I22" s="31" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="J22" s="31"/>
     </row>
@@ -8017,13 +8017,13 @@
         <v>1</v>
       </c>
       <c r="B23" s="37" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D23" s="37" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="E23" s="37" t="s">
         <v>68</v>
@@ -8036,17 +8036,17 @@
         <v>21</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="E24" s="31" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="F24" s="30"/>
       <c r="G24" s="31" t="s">
         <v>618</v>
       </c>
       <c r="I24" s="31" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -8062,13 +8062,13 @@
         <v>21</v>
       </c>
       <c r="D25" s="31" t="s">
+        <v>868</v>
+      </c>
+      <c r="E25" s="31" t="s">
+        <v>719</v>
+      </c>
+      <c r="F25" s="31" t="s">
         <v>871</v>
-      </c>
-      <c r="E25" s="31" t="s">
-        <v>720</v>
-      </c>
-      <c r="F25" s="31" t="s">
-        <v>874</v>
       </c>
       <c r="G25" s="31" t="s">
         <v>619</v>
@@ -8093,7 +8093,7 @@
       <c r="P25" s="4"/>
       <c r="Q25" s="3"/>
       <c r="R25" s="31" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -8101,10 +8101,10 @@
         <v>21</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="E26" s="31" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="F26" s="30"/>
       <c r="G26" s="31" t="s">
@@ -8120,17 +8120,17 @@
         <v>21</v>
       </c>
       <c r="D27" s="31" t="s">
+        <v>807</v>
+      </c>
+      <c r="E27" s="31" t="s">
         <v>808</v>
-      </c>
-      <c r="E27" s="31" t="s">
-        <v>809</v>
       </c>
       <c r="F27" s="30"/>
       <c r="G27" s="30" t="s">
         <v>104</v>
       </c>
       <c r="I27" s="31" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="J27" s="31"/>
     </row>
@@ -8139,13 +8139,13 @@
         <v>1</v>
       </c>
       <c r="B28" s="37" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="C28" s="37" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D28" s="37" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="E28" s="37" t="s">
         <v>68</v>
@@ -8158,17 +8158,17 @@
         <v>21</v>
       </c>
       <c r="D29" s="31" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="E29" s="31" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="F29" s="30"/>
       <c r="G29" s="31" t="s">
         <v>618</v>
       </c>
       <c r="I29" s="31" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
@@ -8184,13 +8184,13 @@
         <v>21</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="E30" s="31" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="F30" s="31" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
       <c r="G30" s="31" t="s">
         <v>619</v>
@@ -8215,7 +8215,7 @@
       <c r="P30" s="4"/>
       <c r="Q30" s="3"/>
       <c r="R30" s="31" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
@@ -8223,10 +8223,10 @@
         <v>21</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="E31" s="31" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="F31" s="30"/>
       <c r="G31" s="31" t="s">
@@ -8242,17 +8242,17 @@
         <v>21</v>
       </c>
       <c r="D32" s="31" t="s">
+        <v>807</v>
+      </c>
+      <c r="E32" s="31" t="s">
         <v>808</v>
-      </c>
-      <c r="E32" s="31" t="s">
-        <v>809</v>
       </c>
       <c r="F32" s="30"/>
       <c r="G32" s="30" t="s">
         <v>104</v>
       </c>
       <c r="I32" s="31" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="J32" s="31"/>
     </row>
@@ -8261,13 +8261,13 @@
         <v>1</v>
       </c>
       <c r="B33" s="37" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C33" s="37" t="s">
+        <v>723</v>
+      </c>
+      <c r="D33" s="37" t="s">
         <v>724</v>
-      </c>
-      <c r="D33" s="37" t="s">
-        <v>725</v>
       </c>
       <c r="E33" s="37" t="s">
         <v>68</v>
@@ -8280,10 +8280,10 @@
         <v>21</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="E34" s="31" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="G34" s="31" t="s">
         <v>629</v>
@@ -8305,16 +8305,16 @@
         <v>21</v>
       </c>
       <c r="D35" s="31" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="E35" s="31" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="G35" s="31" t="s">
         <v>619</v>
       </c>
       <c r="H35" s="31" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I35" s="4">
         <v>10</v>
@@ -8331,16 +8331,16 @@
         <v>21</v>
       </c>
       <c r="D36" s="31" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="E36" s="31" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="G36" s="31" t="s">
         <v>619</v>
       </c>
       <c r="H36" s="31" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I36" s="4">
         <v>10</v>
@@ -8352,10 +8352,10 @@
         <v>21</v>
       </c>
       <c r="D37" s="31" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E37" s="31" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="G37" s="31" t="s">
         <v>619</v>
@@ -8370,13 +8370,13 @@
         <v>1</v>
       </c>
       <c r="B38" s="37" t="s">
+        <v>838</v>
+      </c>
+      <c r="C38" s="37" t="s">
         <v>839</v>
       </c>
-      <c r="C38" s="37" t="s">
+      <c r="D38" s="37" t="s">
         <v>840</v>
-      </c>
-      <c r="D38" s="37" t="s">
-        <v>841</v>
       </c>
       <c r="E38" s="37" t="s">
         <v>68</v>
@@ -8389,10 +8389,10 @@
         <v>21</v>
       </c>
       <c r="D39" s="46" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E39" s="46" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="G39" s="31" t="s">
         <v>619</v>
@@ -8418,7 +8418,7 @@
         <v>0.5</v>
       </c>
       <c r="R39" s="31" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
@@ -8426,10 +8426,10 @@
         <v>21</v>
       </c>
       <c r="D40" s="46" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="E40" s="46" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="G40" s="31" t="s">
         <v>619</v>
@@ -8455,7 +8455,7 @@
         <v>0.5</v>
       </c>
       <c r="R40" s="31" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
     </row>
     <row r="41" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -8463,13 +8463,13 @@
         <v>1</v>
       </c>
       <c r="B41" s="37" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C41" s="37" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="D41" s="37" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E41" s="37" t="s">
         <v>68</v>
@@ -8482,10 +8482,10 @@
         <v>22</v>
       </c>
       <c r="D42" s="31" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E42" s="31" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="G42" s="31" t="s">
         <v>619</v>
@@ -8510,7 +8510,7 @@
       <c r="O42" s="3"/>
       <c r="Q42" s="39"/>
       <c r="R42" s="2" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
     </row>
     <row r="43" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -8518,13 +8518,13 @@
         <v>1</v>
       </c>
       <c r="B43" s="37" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C43" s="37" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="D43" s="37" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E43" s="37" t="s">
         <v>68</v>
@@ -8537,10 +8537,10 @@
         <v>22</v>
       </c>
       <c r="D44" s="31" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="E44" s="31" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="G44" s="31" t="s">
         <v>619</v>
@@ -8565,7 +8565,7 @@
       <c r="O44" s="3"/>
       <c r="Q44" s="39"/>
       <c r="R44" s="2" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
     </row>
     <row r="45" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -8573,13 +8573,13 @@
         <v>1</v>
       </c>
       <c r="B45" s="37" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="C45" s="37" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="D45" s="37" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E45" s="37" t="s">
         <v>68</v>
@@ -8592,10 +8592,10 @@
         <v>22</v>
       </c>
       <c r="D46" s="31" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E46" s="31" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="G46" s="31" t="s">
         <v>619</v>
@@ -8620,7 +8620,7 @@
       <c r="O46" s="3"/>
       <c r="Q46" s="39"/>
       <c r="R46" s="2" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
     </row>
     <row r="47" spans="1:18" s="47" customFormat="1" x14ac:dyDescent="0.25">
@@ -8628,13 +8628,13 @@
         <v>1</v>
       </c>
       <c r="B47" s="47" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="C47" s="47" t="s">
+        <v>803</v>
+      </c>
+      <c r="D47" s="47" t="s">
         <v>804</v>
-      </c>
-      <c r="D47" s="47" t="s">
-        <v>805</v>
       </c>
       <c r="E47" s="47" t="s">
         <v>68</v>
@@ -8648,13 +8648,13 @@
         <v>1</v>
       </c>
       <c r="B48" s="37" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C48" s="37" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D48" s="37" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E48" s="37" t="s">
         <v>68</v>
@@ -8667,13 +8667,13 @@
         <v>1</v>
       </c>
       <c r="B49" s="37" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C49" s="37" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="D49" s="37" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E49" s="37" t="s">
         <v>68</v>
@@ -8686,7 +8686,7 @@
         <v>1</v>
       </c>
       <c r="B50" s="37" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C50" s="37" t="s">
         <v>74</v>
@@ -8714,7 +8714,7 @@
         <v>619</v>
       </c>
       <c r="H51" s="31" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="I51" s="31">
         <v>0</v>
@@ -8733,13 +8733,13 @@
         <v>1</v>
       </c>
       <c r="B52" s="47" t="s">
+        <v>765</v>
+      </c>
+      <c r="C52" s="47" t="s">
+        <v>752</v>
+      </c>
+      <c r="D52" s="47" t="s">
         <v>766</v>
-      </c>
-      <c r="C52" s="47" t="s">
-        <v>753</v>
-      </c>
-      <c r="D52" s="47" t="s">
-        <v>767</v>
       </c>
       <c r="E52" s="47" t="s">
         <v>68</v>
@@ -8753,10 +8753,10 @@
         <v>21</v>
       </c>
       <c r="D53" s="31" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="E53" s="31" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="G53" s="31" t="s">
         <v>619</v>
@@ -8778,10 +8778,10 @@
         <v>21</v>
       </c>
       <c r="D54" s="31" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="E54" s="31" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="G54" s="31" t="s">
         <v>619</v>
@@ -8803,10 +8803,10 @@
         <v>21</v>
       </c>
       <c r="D55" s="31" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="E55" s="31" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="G55" s="31" t="s">
         <v>619</v>
@@ -8828,10 +8828,10 @@
         <v>21</v>
       </c>
       <c r="D56" s="31" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="E56" s="31" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="G56" s="31" t="s">
         <v>619</v>
@@ -8853,13 +8853,13 @@
         <v>1</v>
       </c>
       <c r="B57" s="37" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="C57" s="37" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="D57" s="37" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E57" s="37" t="s">
         <v>68</v>
@@ -8872,10 +8872,10 @@
         <v>21</v>
       </c>
       <c r="D58" s="31" t="s">
+        <v>768</v>
+      </c>
+      <c r="E58" s="31" t="s">
         <v>769</v>
-      </c>
-      <c r="E58" s="31" t="s">
-        <v>770</v>
       </c>
       <c r="G58" s="31" t="s">
         <v>619</v>
@@ -8897,13 +8897,13 @@
         <v>1</v>
       </c>
       <c r="B59" s="37" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="C59" s="37" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="D59" s="37" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E59" s="37" t="s">
         <v>68</v>
@@ -8916,10 +8916,10 @@
         <v>22</v>
       </c>
       <c r="D60" s="31" t="s">
+        <v>771</v>
+      </c>
+      <c r="E60" s="31" t="s">
         <v>772</v>
-      </c>
-      <c r="E60" s="31" t="s">
-        <v>773</v>
       </c>
       <c r="G60" s="31" t="s">
         <v>619</v>
@@ -8944,7 +8944,7 @@
       <c r="O60" s="3"/>
       <c r="Q60" s="39"/>
       <c r="R60" s="2" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
     </row>
     <row r="61" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -8952,13 +8952,13 @@
         <v>1</v>
       </c>
       <c r="B61" s="37" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="C61" s="37" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="D61" s="37" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E61" s="37" t="s">
         <v>68</v>
@@ -8971,10 +8971,10 @@
         <v>22</v>
       </c>
       <c r="D62" s="31" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="E62" s="31" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="G62" s="31" t="s">
         <v>619</v>
@@ -8999,7 +8999,7 @@
       <c r="O62" s="3"/>
       <c r="Q62" s="39"/>
       <c r="R62" s="2" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
     </row>
     <row r="63" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -9007,13 +9007,13 @@
         <v>1</v>
       </c>
       <c r="B63" s="37" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C63" s="37" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D63" s="37" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E63" s="37" t="s">
         <v>68</v>
@@ -9026,10 +9026,10 @@
         <v>22</v>
       </c>
       <c r="D64" s="31" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="E64" s="31" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="G64" s="31" t="s">
         <v>619</v>
@@ -9054,7 +9054,7 @@
       <c r="O64" s="3"/>
       <c r="Q64" s="39"/>
       <c r="R64" s="2" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
     </row>
     <row r="65" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -9062,13 +9062,13 @@
         <v>1</v>
       </c>
       <c r="B65" s="37" t="s">
+        <v>797</v>
+      </c>
+      <c r="C65" s="37" t="s">
         <v>798</v>
       </c>
-      <c r="C65" s="37" t="s">
-        <v>799</v>
-      </c>
       <c r="D65" s="37" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E65" s="37" t="s">
         <v>68</v>
@@ -9081,10 +9081,10 @@
         <v>22</v>
       </c>
       <c r="D66" s="31" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E66" s="31" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="G66" s="31" t="s">
         <v>619</v>
@@ -9109,7 +9109,7 @@
       <c r="O66" s="3"/>
       <c r="Q66" s="39"/>
       <c r="R66" s="2" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
     </row>
     <row r="67" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -9117,13 +9117,13 @@
         <v>1</v>
       </c>
       <c r="B67" s="37" t="s">
+        <v>791</v>
+      </c>
+      <c r="C67" s="37" t="s">
+        <v>793</v>
+      </c>
+      <c r="D67" s="37" t="s">
         <v>792</v>
-      </c>
-      <c r="C67" s="37" t="s">
-        <v>794</v>
-      </c>
-      <c r="D67" s="37" t="s">
-        <v>793</v>
       </c>
       <c r="E67" s="37" t="s">
         <v>68</v>
@@ -9136,10 +9136,10 @@
         <v>22</v>
       </c>
       <c r="D68" s="31" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E68" s="31" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="G68" s="31" t="s">
         <v>619</v>
@@ -9164,7 +9164,7 @@
       <c r="O68" s="3"/>
       <c r="Q68" s="39"/>
       <c r="R68" s="2" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
     </row>
     <row r="69" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -9172,13 +9172,13 @@
         <v>1</v>
       </c>
       <c r="B69" s="37" t="s">
+        <v>784</v>
+      </c>
+      <c r="C69" s="37" t="s">
+        <v>786</v>
+      </c>
+      <c r="D69" s="37" t="s">
         <v>785</v>
-      </c>
-      <c r="C69" s="37" t="s">
-        <v>787</v>
-      </c>
-      <c r="D69" s="37" t="s">
-        <v>786</v>
       </c>
       <c r="E69" s="37" t="s">
         <v>68</v>
@@ -9191,10 +9191,10 @@
         <v>21</v>
       </c>
       <c r="D70" s="31" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E70" s="31" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="G70" s="31" t="s">
         <v>619</v>
@@ -9216,10 +9216,10 @@
         <v>21</v>
       </c>
       <c r="D71" s="31" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="E71" s="31" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="G71" s="31" t="s">
         <v>619</v>
@@ -9241,13 +9241,13 @@
         <v>1</v>
       </c>
       <c r="B72" s="37" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="C72" s="37" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D72" s="37" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E72" s="37" t="s">
         <v>68</v>
@@ -9260,13 +9260,13 @@
         <v>1</v>
       </c>
       <c r="B73" s="37" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="C73" s="37" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="D73" s="37" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="E73" s="37" t="s">
         <v>68</v>
@@ -9279,13 +9279,13 @@
         <v>1</v>
       </c>
       <c r="B74" s="37" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="C74" s="37" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="D74" s="37" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E74" s="37" t="s">
         <v>68</v>
@@ -9298,13 +9298,13 @@
         <v>1</v>
       </c>
       <c r="B75" s="37" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C75" s="37" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="D75" s="37" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="E75" s="37" t="s">
         <v>68</v>
@@ -9317,13 +9317,13 @@
         <v>1</v>
       </c>
       <c r="B76" s="37" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="C76" s="37" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="D76" s="37" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E76" s="37" t="s">
         <v>68</v>
@@ -9336,13 +9336,13 @@
         <v>1</v>
       </c>
       <c r="B77" s="37" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C77" s="37" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="D77" s="37" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E77" s="37" t="s">
         <v>68</v>
@@ -9355,13 +9355,13 @@
         <v>1</v>
       </c>
       <c r="B78" s="37" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="C78" s="37" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="D78" s="37" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E78" s="37" t="s">
         <v>68</v>
@@ -9374,13 +9374,13 @@
         <v>1</v>
       </c>
       <c r="B79" s="37" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="C79" s="37" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="D79" s="37" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="E79" s="37" t="s">
         <v>68</v>
@@ -9393,13 +9393,13 @@
         <v>1</v>
       </c>
       <c r="B80" s="37" t="s">
+        <v>809</v>
+      </c>
+      <c r="C80" s="37" t="s">
         <v>810</v>
       </c>
-      <c r="C80" s="37" t="s">
+      <c r="D80" s="37" t="s">
         <v>811</v>
-      </c>
-      <c r="D80" s="37" t="s">
-        <v>812</v>
       </c>
       <c r="E80" s="37" t="s">
         <v>68</v>
@@ -9412,13 +9412,13 @@
         <v>1</v>
       </c>
       <c r="B81" s="37" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="C81" s="37" t="s">
-        <v>901</v>
+        <v>898</v>
       </c>
       <c r="D81" s="37" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
       <c r="E81" s="37" t="s">
         <v>68</v>
@@ -9431,10 +9431,10 @@
         <v>21</v>
       </c>
       <c r="D82" s="46" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
       <c r="E82" s="46" t="s">
-        <v>903</v>
+        <v>900</v>
       </c>
       <c r="G82" s="31" t="s">
         <v>619</v>
@@ -9460,7 +9460,7 @@
         <v>0.5</v>
       </c>
       <c r="R82" s="31" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.25">
@@ -9468,10 +9468,10 @@
         <v>21</v>
       </c>
       <c r="D83" s="46" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="E83" s="46" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="G83" s="31" t="s">
         <v>619</v>
@@ -9497,7 +9497,7 @@
         <v>0.5</v>
       </c>
       <c r="R83" s="31" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.25">
@@ -9505,10 +9505,10 @@
         <v>22</v>
       </c>
       <c r="D84" s="46" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="E84" s="46" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="G84" s="31" t="s">
         <v>619</v>
@@ -9534,7 +9534,7 @@
         <v>0.5</v>
       </c>
       <c r="R84" s="31" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.25">
@@ -9542,10 +9542,10 @@
         <v>22</v>
       </c>
       <c r="D85" s="46" t="s">
-        <v>910</v>
+        <v>907</v>
       </c>
       <c r="E85" s="46" t="s">
-        <v>909</v>
+        <v>906</v>
       </c>
       <c r="G85" s="31" t="s">
         <v>619</v>
@@ -9571,7 +9571,7 @@
         <v>0.5</v>
       </c>
       <c r="R85" s="31" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
     </row>
     <row r="86" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -9579,13 +9579,13 @@
         <v>0</v>
       </c>
       <c r="B86" s="37" t="s">
+        <v>846</v>
+      </c>
+      <c r="C86" s="37" t="s">
+        <v>845</v>
+      </c>
+      <c r="D86" s="37" t="s">
         <v>847</v>
-      </c>
-      <c r="C86" s="37" t="s">
-        <v>846</v>
-      </c>
-      <c r="D86" s="37" t="s">
-        <v>848</v>
       </c>
       <c r="E86" s="37" t="s">
         <v>233</v>
@@ -9870,7 +9870,7 @@
         <v>459</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C2" s="44" t="s">
         <v>635</v>
@@ -9909,7 +9909,7 @@
         <v>627</v>
       </c>
       <c r="B3" s="51" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C3" s="44" t="s">
         <v>640</v>
@@ -9948,7 +9948,7 @@
         <v>642</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="C4" s="40" t="s">
         <v>636</v>
@@ -9981,7 +9981,7 @@
         <v>643</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="C5" s="40" t="s">
         <v>637</v>
@@ -10014,7 +10014,7 @@
         <v>644</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="C6" s="40" t="s">
         <v>639</v>
@@ -10047,7 +10047,7 @@
         <v>645</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="C7" s="40" t="s">
         <v>638</v>
@@ -10077,12 +10077,12 @@
     </row>
     <row r="8" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="40" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B8" s="30"/>
       <c r="C8" s="40"/>
       <c r="D8" s="40" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="E8" s="40" t="s">
         <v>468</v>
@@ -10106,12 +10106,12 @@
     </row>
     <row r="9" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="40" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="40"/>
       <c r="D9" s="40" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="E9" s="40" t="s">
         <v>468</v>
@@ -10135,12 +10135,12 @@
     </row>
     <row r="10" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="40" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B10" s="30"/>
       <c r="C10" s="40"/>
       <c r="D10" s="40" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="E10" s="40" t="s">
         <v>468</v>
@@ -10164,12 +10164,12 @@
     </row>
     <row r="11" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="40" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B11" s="30"/>
       <c r="C11" s="40"/>
       <c r="D11" s="40" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="E11" s="40" t="s">
         <v>468</v>
@@ -10193,12 +10193,12 @@
     </row>
     <row r="12" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="40" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B12" s="30"/>
       <c r="C12" s="40"/>
       <c r="D12" s="40" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="E12" s="40" t="s">
         <v>468</v>
@@ -10222,12 +10222,12 @@
     </row>
     <row r="13" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="40" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B13" s="30"/>
       <c r="C13" s="40"/>
       <c r="D13" s="40" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E13" s="40" t="s">
         <v>468</v>
@@ -10251,12 +10251,12 @@
     </row>
     <row r="14" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="40" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B14" s="30"/>
       <c r="C14" s="40"/>
       <c r="D14" s="40" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="E14" s="40" t="s">
         <v>468</v>
@@ -10280,12 +10280,12 @@
     </row>
     <row r="15" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="40" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B15" s="30"/>
       <c r="C15" s="40"/>
       <c r="D15" s="40" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="E15" s="40" t="s">
         <v>468</v>
@@ -10309,12 +10309,12 @@
     </row>
     <row r="16" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="40" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B16" s="30"/>
       <c r="C16" s="40"/>
       <c r="D16" s="40" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="E16" s="40" t="s">
         <v>468</v>
@@ -10338,12 +10338,12 @@
     </row>
     <row r="17" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="40" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B17" s="30"/>
       <c r="C17" s="40"/>
       <c r="D17" s="40" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E17" s="40" t="s">
         <v>468</v>
@@ -10367,12 +10367,12 @@
     </row>
     <row r="18" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="40" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B18" s="30"/>
       <c r="C18" s="40"/>
       <c r="D18" s="40" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E18" s="40" t="s">
         <v>468</v>
@@ -10396,12 +10396,12 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="40" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B19" s="30"/>
       <c r="C19" s="40"/>
       <c r="D19" s="40" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E19" s="40" t="s">
         <v>468</v>
@@ -10425,12 +10425,12 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="40" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B20" s="30"/>
       <c r="C20" s="40"/>
       <c r="D20" s="40" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E20" s="40" t="s">
         <v>468</v>
@@ -10454,12 +10454,12 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="40" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B21" s="30"/>
       <c r="C21" s="40"/>
       <c r="D21" s="40" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="E21" s="40" t="s">
         <v>468</v>
@@ -10483,15 +10483,15 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="40" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B22" s="30"/>
       <c r="C22" s="40"/>
       <c r="D22" s="40" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="E22" s="40" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="F22" s="40" t="s">
         <v>64</v>
@@ -10512,15 +10512,15 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="40" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B23" s="30"/>
       <c r="C23" s="40"/>
       <c r="D23" s="40" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E23" s="40" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="F23" s="40" t="s">
         <v>64</v>
@@ -10541,15 +10541,15 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="40" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B24" s="30"/>
       <c r="C24" s="40"/>
       <c r="D24" s="40" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="E24" s="40" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="F24" s="40" t="s">
         <v>64</v>
@@ -10570,17 +10570,17 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="40" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B25" s="40" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C25" s="40"/>
       <c r="D25" s="40" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="E25" s="40" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="F25" s="40" t="s">
         <v>64</v>
@@ -10601,17 +10601,17 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="40" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B26" s="40" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C26" s="40"/>
       <c r="D26" s="40" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E26" s="40" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="F26" s="40" t="s">
         <v>64</v>
@@ -10632,17 +10632,17 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="40" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B27" s="40" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="C27" s="40"/>
       <c r="D27" s="40" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="E27" s="40" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="F27" s="40" t="s">
         <v>64</v>
@@ -10663,17 +10663,17 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="40" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B28" s="40" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="C28" s="40"/>
       <c r="D28" s="40" t="s">
+        <v>669</v>
+      </c>
+      <c r="E28" s="40" t="s">
         <v>670</v>
-      </c>
-      <c r="E28" s="40" t="s">
-        <v>671</v>
       </c>
       <c r="F28" s="40" t="s">
         <v>64</v>
@@ -10694,17 +10694,17 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="40" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B29" s="40" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C29" s="40"/>
       <c r="D29" s="40" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="E29" s="40" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="F29" s="40" t="s">
         <v>64</v>
@@ -10725,17 +10725,17 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="40" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B30" s="40" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="C30" s="40"/>
       <c r="D30" s="40" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="E30" s="40" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="F30" s="40" t="s">
         <v>64</v>
@@ -10756,17 +10756,17 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="40" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B31" s="40" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="C31" s="40"/>
       <c r="D31" s="40" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="E31" s="40" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="F31" s="40" t="s">
         <v>64</v>
@@ -10787,14 +10787,14 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="40" t="s">
-        <v>898</v>
+        <v>895</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>898</v>
+        <v>895</v>
       </c>
       <c r="C32" s="40"/>
       <c r="D32" s="40" t="s">
-        <v>899</v>
+        <v>896</v>
       </c>
       <c r="E32" s="40"/>
       <c r="F32" s="40" t="s">
@@ -19655,7 +19655,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>557</v>

</xml_diff>

<commit_message>
updated test spreadsheet for blend branch
These should be ready to run, but need some testing. I can merge back to
master in morning, but wanted to see if anyone was running anything. Old
spreadsheets may not work anymore.
</commit_message>
<xml_diff>
--- a/projects/dfg_test_m0_office_blend.xlsx
+++ b/projects/dfg_test_m0_office_blend.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="2880" windowWidth="21210" windowHeight="2895" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="2940" windowWidth="21210" windowHeight="2835" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$AA$64</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$AA$65</definedName>
     <definedName name="AnalysisType">Lookups!$A$17:$A$23</definedName>
     <definedName name="instance_defs">Lookups!$A$2:$D$9</definedName>
     <definedName name="instance_types">Lookups!$A$2:$A$9</definedName>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2536" uniqueCount="916">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2541" uniqueCount="919">
   <si>
     <t>type</t>
   </si>
@@ -2767,21 +2767,9 @@
     <t>Shift Hours of Operation</t>
   </si>
   <si>
-    <t>NationalGrid office reduced crash</t>
-  </si>
-  <si>
     <t>single_run</t>
   </si>
   <si>
-    <t>Blend A</t>
-  </si>
-  <si>
-    <t>Blend B</t>
-  </si>
-  <si>
-    <t>Blend C</t>
-  </si>
-  <si>
     <t>dgoldwas</t>
   </si>
   <si>
@@ -2789,6 +2777,27 @@
   </si>
   <si>
     <t>../../../GitHub/cofee-measures/lib/</t>
+  </si>
+  <si>
+    <t>Office BlendA</t>
+  </si>
+  <si>
+    <t>Office BlendB</t>
+  </si>
+  <si>
+    <t>Office BlendC</t>
+  </si>
+  <si>
+    <t>Envelope Zoning Logic</t>
+  </si>
+  <si>
+    <t>zoning_logic</t>
+  </si>
+  <si>
+    <t>Each SpaceType on at Least One Story</t>
+  </si>
+  <si>
+    <t>NationalGrid office blend</t>
   </si>
 </sst>
 </file>
@@ -7013,8 +7022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7061,7 +7070,7 @@
         <v>456</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>457</v>
@@ -7154,7 +7163,7 @@
         <v>39</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>908</v>
+        <v>918</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>471</v>
@@ -7165,7 +7174,7 @@
         <v>25</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>914</v>
+        <v>910</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>660</v>
@@ -7244,7 +7253,7 @@
         <v>451</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -7403,7 +7412,7 @@
         <v>733</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>915</v>
+        <v>911</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -7442,11 +7451,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z140"/>
+  <dimension ref="A1:Z141"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7801,7 +7810,7 @@
         <v>618</v>
       </c>
       <c r="I14" s="31" t="s">
-        <v>910</v>
+        <v>912</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -7924,7 +7933,7 @@
         <v>618</v>
       </c>
       <c r="I19" s="31" t="s">
-        <v>911</v>
+        <v>913</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -8074,21 +8083,21 @@
         <v>619</v>
       </c>
       <c r="I25" s="4">
-        <v>0.1</v>
+        <v>0.04</v>
       </c>
       <c r="J25" s="3"/>
       <c r="K25" s="3">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="L25" s="3">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="M25" s="3">
-        <v>0.1</v>
+        <v>0.04</v>
       </c>
       <c r="N25" s="31">
         <f>(K25+L25)/6</f>
-        <v>3.3333333333333333E-2</v>
+        <v>0.02</v>
       </c>
       <c r="P25" s="4"/>
       <c r="Q25" s="3"/>
@@ -8168,7 +8177,7 @@
         <v>618</v>
       </c>
       <c r="I29" s="31" t="s">
-        <v>912</v>
+        <v>914</v>
       </c>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
@@ -8196,7 +8205,7 @@
         <v>619</v>
       </c>
       <c r="I30" s="4">
-        <v>0.17499999999999999</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="J30" s="3"/>
       <c r="K30" s="3">
@@ -8365,91 +8374,72 @@
       </c>
       <c r="J37" s="31"/>
     </row>
-    <row r="38" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="37" t="b">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B38" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" s="31" t="s">
+        <v>915</v>
+      </c>
+      <c r="E38" s="31" t="s">
+        <v>916</v>
+      </c>
+      <c r="G38" s="31" t="s">
+        <v>618</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>917</v>
+      </c>
+      <c r="J38" s="31"/>
+    </row>
+    <row r="39" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B38" s="37" t="s">
+      <c r="B39" s="37" t="s">
         <v>838</v>
       </c>
-      <c r="C38" s="37" t="s">
+      <c r="C39" s="37" t="s">
         <v>839</v>
       </c>
-      <c r="D38" s="37" t="s">
+      <c r="D39" s="37" t="s">
         <v>840</v>
       </c>
-      <c r="E38" s="37" t="s">
+      <c r="E39" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="H38" s="38"/>
-      <c r="I38" s="38"/>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B39" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D39" s="46" t="s">
-        <v>760</v>
-      </c>
-      <c r="E39" s="46" t="s">
-        <v>762</v>
-      </c>
-      <c r="G39" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="I39" s="4">
-        <v>8</v>
-      </c>
-      <c r="J39" s="31"/>
-      <c r="K39" s="31">
-        <v>7</v>
-      </c>
-      <c r="L39" s="31">
-        <v>10</v>
-      </c>
-      <c r="M39" s="31">
-        <v>8</v>
-      </c>
-      <c r="N39" s="31">
-        <f>(K39+L39)/6</f>
-        <v>2.8333333333333335</v>
-      </c>
-      <c r="O39" s="31">
-        <v>0.5</v>
-      </c>
-      <c r="R39" s="31" t="s">
-        <v>874</v>
-      </c>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B40" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D40" s="46" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E40" s="46" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="G40" s="31" t="s">
         <v>619</v>
       </c>
       <c r="I40" s="4">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="J40" s="31"/>
       <c r="K40" s="31">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="L40" s="31">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="M40" s="31">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="N40" s="31">
         <f>(K40+L40)/6</f>
-        <v>6</v>
+        <v>2.8333333333333335</v>
       </c>
       <c r="O40" s="31">
         <v>0.5</v>
@@ -8458,222 +8448,240 @@
         <v>874</v>
       </c>
     </row>
-    <row r="41" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="37" t="b">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B41" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" s="46" t="s">
+        <v>761</v>
+      </c>
+      <c r="E41" s="46" t="s">
+        <v>763</v>
+      </c>
+      <c r="G41" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="I41" s="4">
+        <v>17</v>
+      </c>
+      <c r="J41" s="31"/>
+      <c r="K41" s="31">
+        <v>16</v>
+      </c>
+      <c r="L41" s="31">
+        <v>20</v>
+      </c>
+      <c r="M41" s="31">
+        <v>17</v>
+      </c>
+      <c r="N41" s="31">
+        <f>(K41+L41)/6</f>
+        <v>6</v>
+      </c>
+      <c r="O41" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="R41" s="31" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B41" s="37" t="s">
+      <c r="B42" s="37" t="s">
         <v>743</v>
       </c>
-      <c r="C41" s="37" t="s">
+      <c r="C42" s="37" t="s">
         <v>742</v>
       </c>
-      <c r="D41" s="37" t="s">
+      <c r="D42" s="37" t="s">
         <v>734</v>
       </c>
-      <c r="E41" s="37" t="s">
+      <c r="E42" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="H41" s="38"/>
-      <c r="I41" s="38"/>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B42" s="31" t="s">
+      <c r="H42" s="38"/>
+      <c r="I42" s="38"/>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B43" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D42" s="31" t="s">
+      <c r="D43" s="31" t="s">
         <v>745</v>
       </c>
-      <c r="E42" s="31" t="s">
+      <c r="E43" s="31" t="s">
         <v>744</v>
       </c>
-      <c r="G42" s="31" t="s">
+      <c r="G43" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="I42" s="31">
+      <c r="I43" s="31">
         <v>1.55</v>
       </c>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3">
+      <c r="J43" s="3"/>
+      <c r="K43" s="3">
         <v>0.1</v>
       </c>
-      <c r="L42" s="3">
+      <c r="L43" s="3">
         <v>3</v>
       </c>
-      <c r="M42" s="3">
+      <c r="M43" s="3">
         <v>1</v>
       </c>
-      <c r="N42" s="31">
-        <f>(K42+L42)/6</f>
+      <c r="N43" s="31">
+        <f>(K43+L43)/6</f>
         <v>0.51666666666666672</v>
       </c>
-      <c r="O42" s="3"/>
-      <c r="Q42" s="39"/>
-      <c r="R42" s="2" t="s">
+      <c r="O43" s="3"/>
+      <c r="Q43" s="39"/>
+      <c r="R43" s="2" t="s">
         <v>874</v>
       </c>
     </row>
-    <row r="43" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="37" t="b">
+    <row r="44" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B43" s="37" t="s">
+      <c r="B44" s="37" t="s">
         <v>749</v>
       </c>
-      <c r="C43" s="37" t="s">
+      <c r="C44" s="37" t="s">
         <v>751</v>
       </c>
-      <c r="D43" s="37" t="s">
+      <c r="D44" s="37" t="s">
         <v>735</v>
       </c>
-      <c r="E43" s="37" t="s">
+      <c r="E44" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="H43" s="38"/>
-      <c r="I43" s="38"/>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B44" s="31" t="s">
+      <c r="H44" s="38"/>
+      <c r="I44" s="38"/>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B45" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D44" s="31" t="s">
+      <c r="D45" s="31" t="s">
         <v>747</v>
       </c>
-      <c r="E44" s="31" t="s">
+      <c r="E45" s="31" t="s">
         <v>746</v>
       </c>
-      <c r="G44" s="31" t="s">
+      <c r="G45" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="I44" s="31">
+      <c r="I45" s="31">
         <v>1.55</v>
       </c>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3">
+      <c r="J45" s="3"/>
+      <c r="K45" s="3">
         <v>0.1</v>
       </c>
-      <c r="L44" s="3">
+      <c r="L45" s="3">
         <v>3</v>
       </c>
-      <c r="M44" s="3">
+      <c r="M45" s="3">
         <v>1</v>
       </c>
-      <c r="N44" s="31">
-        <f>(K44+L44)/6</f>
+      <c r="N45" s="31">
+        <f>(K45+L45)/6</f>
         <v>0.51666666666666672</v>
       </c>
-      <c r="O44" s="3"/>
-      <c r="Q44" s="39"/>
-      <c r="R44" s="2" t="s">
+      <c r="O45" s="3"/>
+      <c r="Q45" s="39"/>
+      <c r="R45" s="2" t="s">
         <v>874</v>
       </c>
     </row>
-    <row r="45" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="37" t="b">
+    <row r="46" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B45" s="37" t="s">
+      <c r="B46" s="37" t="s">
         <v>748</v>
       </c>
-      <c r="C45" s="37" t="s">
+      <c r="C46" s="37" t="s">
         <v>750</v>
       </c>
-      <c r="D45" s="37" t="s">
+      <c r="D46" s="37" t="s">
         <v>736</v>
       </c>
-      <c r="E45" s="37" t="s">
+      <c r="E46" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="H45" s="38"/>
-      <c r="I45" s="38"/>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B46" s="31" t="s">
+      <c r="H46" s="38"/>
+      <c r="I46" s="38"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B47" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D46" s="31" t="s">
+      <c r="D47" s="31" t="s">
         <v>758</v>
       </c>
-      <c r="E46" s="31" t="s">
+      <c r="E47" s="31" t="s">
         <v>757</v>
       </c>
-      <c r="G46" s="31" t="s">
+      <c r="G47" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="I46" s="31">
+      <c r="I47" s="31">
         <v>1.55</v>
       </c>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3">
+      <c r="J47" s="3"/>
+      <c r="K47" s="3">
         <v>0.1</v>
       </c>
-      <c r="L46" s="3">
+      <c r="L47" s="3">
         <v>3</v>
       </c>
-      <c r="M46" s="3">
+      <c r="M47" s="3">
         <v>1</v>
       </c>
-      <c r="N46" s="31">
-        <f>(K46+L46)/6</f>
+      <c r="N47" s="31">
+        <f>(K47+L47)/6</f>
         <v>0.51666666666666672</v>
       </c>
-      <c r="O46" s="3"/>
-      <c r="Q46" s="39"/>
-      <c r="R46" s="2" t="s">
+      <c r="O47" s="3"/>
+      <c r="Q47" s="39"/>
+      <c r="R47" s="2" t="s">
         <v>874</v>
       </c>
     </row>
-    <row r="47" spans="1:18" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="47" t="b">
+    <row r="48" spans="1:18" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="B47" s="47" t="s">
+      <c r="B48" s="47" t="s">
         <v>805</v>
       </c>
-      <c r="C47" s="47" t="s">
+      <c r="C48" s="47" t="s">
         <v>803</v>
       </c>
-      <c r="D47" s="47" t="s">
+      <c r="D48" s="47" t="s">
         <v>804</v>
       </c>
-      <c r="E47" s="47" t="s">
+      <c r="E48" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="F47" s="37"/>
-      <c r="H47" s="48"/>
-      <c r="I47" s="48"/>
-    </row>
-    <row r="48" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="B48" s="37" t="s">
-        <v>806</v>
-      </c>
-      <c r="C48" s="37" t="s">
-        <v>802</v>
-      </c>
-      <c r="D48" s="37" t="s">
-        <v>801</v>
-      </c>
-      <c r="E48" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="H48" s="38"/>
-      <c r="I48" s="38"/>
+      <c r="F48" s="37"/>
+      <c r="H48" s="48"/>
+      <c r="I48" s="48"/>
     </row>
     <row r="49" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="37" t="b">
         <v>1</v>
       </c>
       <c r="B49" s="37" t="s">
-        <v>759</v>
+        <v>806</v>
       </c>
       <c r="C49" s="37" t="s">
-        <v>841</v>
+        <v>802</v>
       </c>
       <c r="D49" s="37" t="s">
-        <v>737</v>
+        <v>801</v>
       </c>
       <c r="E49" s="37" t="s">
         <v>68</v>
@@ -8686,13 +8694,13 @@
         <v>1</v>
       </c>
       <c r="B50" s="37" t="s">
-        <v>666</v>
+        <v>759</v>
       </c>
       <c r="C50" s="37" t="s">
-        <v>74</v>
+        <v>841</v>
       </c>
       <c r="D50" s="37" t="s">
-        <v>74</v>
+        <v>737</v>
       </c>
       <c r="E50" s="37" t="s">
         <v>68</v>
@@ -8700,88 +8708,82 @@
       <c r="H50" s="38"/>
       <c r="I50" s="38"/>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B51" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D51" s="31" t="s">
+    <row r="51" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B51" s="37" t="s">
+        <v>666</v>
+      </c>
+      <c r="C51" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="D51" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="E51" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="H51" s="38"/>
+      <c r="I51" s="38"/>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B52" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D52" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="E51" s="31" t="s">
+      <c r="E52" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="G51" s="31" t="s">
+      <c r="G52" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="H51" s="31" t="s">
+      <c r="H52" s="31" t="s">
         <v>764</v>
       </c>
-      <c r="I51" s="31">
-        <v>0</v>
-      </c>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
-      <c r="L51" s="3"/>
-      <c r="M51" s="3"/>
-      <c r="N51" s="3"/>
-      <c r="O51" s="3"/>
-      <c r="Q51" s="39"/>
-      <c r="R51" s="2"/>
-    </row>
-    <row r="52" spans="1:18" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="47" t="b">
+      <c r="I52" s="31">
+        <v>0</v>
+      </c>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
+      <c r="N52" s="3"/>
+      <c r="O52" s="3"/>
+      <c r="Q52" s="39"/>
+      <c r="R52" s="2"/>
+    </row>
+    <row r="53" spans="1:18" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="B52" s="47" t="s">
+      <c r="B53" s="47" t="s">
         <v>765</v>
       </c>
-      <c r="C52" s="47" t="s">
+      <c r="C53" s="47" t="s">
         <v>752</v>
       </c>
-      <c r="D52" s="47" t="s">
+      <c r="D53" s="47" t="s">
         <v>766</v>
       </c>
-      <c r="E52" s="47" t="s">
+      <c r="E53" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="F52" s="37"/>
-      <c r="H52" s="48"/>
-      <c r="I52" s="48"/>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B53" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D53" s="31" t="s">
-        <v>844</v>
-      </c>
-      <c r="E53" s="31" t="s">
-        <v>843</v>
-      </c>
-      <c r="G53" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="I53" s="31">
-        <v>1</v>
-      </c>
-      <c r="J53" s="3"/>
-      <c r="K53" s="3"/>
-      <c r="L53" s="3"/>
-      <c r="M53" s="3"/>
-      <c r="N53" s="3"/>
-      <c r="O53" s="3"/>
-      <c r="Q53" s="39"/>
-      <c r="R53" s="2"/>
+      <c r="F53" s="37"/>
+      <c r="H53" s="48"/>
+      <c r="I53" s="48"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B54" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D54" s="31" t="s">
-        <v>849</v>
+        <v>844</v>
       </c>
       <c r="E54" s="31" t="s">
-        <v>848</v>
+        <v>843</v>
       </c>
       <c r="G54" s="31" t="s">
         <v>619</v>
@@ -8803,10 +8805,10 @@
         <v>21</v>
       </c>
       <c r="D55" s="31" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="E55" s="31" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="G55" s="31" t="s">
         <v>619</v>
@@ -8828,10 +8830,10 @@
         <v>21</v>
       </c>
       <c r="D56" s="31" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="E56" s="31" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="G56" s="31" t="s">
         <v>619</v>
@@ -8848,378 +8850,378 @@
       <c r="Q56" s="39"/>
       <c r="R56" s="2"/>
     </row>
-    <row r="57" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="37" t="b">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B57" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D57" s="31" t="s">
+        <v>853</v>
+      </c>
+      <c r="E57" s="31" t="s">
+        <v>852</v>
+      </c>
+      <c r="G57" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="I57" s="31">
         <v>1</v>
       </c>
-      <c r="B57" s="37" t="s">
+      <c r="J57" s="3"/>
+      <c r="K57" s="3"/>
+      <c r="L57" s="3"/>
+      <c r="M57" s="3"/>
+      <c r="N57" s="3"/>
+      <c r="O57" s="3"/>
+      <c r="Q57" s="39"/>
+      <c r="R57" s="2"/>
+    </row>
+    <row r="58" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B58" s="37" t="s">
         <v>767</v>
       </c>
-      <c r="C57" s="37" t="s">
+      <c r="C58" s="37" t="s">
         <v>753</v>
       </c>
-      <c r="D57" s="37" t="s">
+      <c r="D58" s="37" t="s">
         <v>738</v>
       </c>
-      <c r="E57" s="37" t="s">
+      <c r="E58" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="H57" s="38"/>
-      <c r="I57" s="38"/>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B58" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D58" s="31" t="s">
+      <c r="H58" s="38"/>
+      <c r="I58" s="38"/>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B59" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D59" s="31" t="s">
         <v>768</v>
       </c>
-      <c r="E58" s="31" t="s">
+      <c r="E59" s="31" t="s">
         <v>769</v>
       </c>
-      <c r="G58" s="31" t="s">
+      <c r="G59" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="I58" s="31">
+      <c r="I59" s="31">
         <v>1</v>
       </c>
-      <c r="J58" s="3"/>
-      <c r="K58" s="3"/>
-      <c r="L58" s="3"/>
-      <c r="M58" s="3"/>
-      <c r="N58" s="3"/>
-      <c r="O58" s="3"/>
-      <c r="Q58" s="39"/>
-      <c r="R58" s="2"/>
-    </row>
-    <row r="59" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="37" t="b">
+      <c r="J59" s="3"/>
+      <c r="K59" s="3"/>
+      <c r="L59" s="3"/>
+      <c r="M59" s="3"/>
+      <c r="N59" s="3"/>
+      <c r="O59" s="3"/>
+      <c r="Q59" s="39"/>
+      <c r="R59" s="2"/>
+    </row>
+    <row r="60" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B59" s="37" t="s">
+      <c r="B60" s="37" t="s">
         <v>770</v>
       </c>
-      <c r="C59" s="37" t="s">
+      <c r="C60" s="37" t="s">
         <v>754</v>
       </c>
-      <c r="D59" s="37" t="s">
+      <c r="D60" s="37" t="s">
         <v>739</v>
       </c>
-      <c r="E59" s="37" t="s">
+      <c r="E60" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="H59" s="38"/>
-      <c r="I59" s="38"/>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B60" s="31" t="s">
+      <c r="H60" s="38"/>
+      <c r="I60" s="38"/>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B61" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D60" s="31" t="s">
+      <c r="D61" s="31" t="s">
         <v>771</v>
       </c>
-      <c r="E60" s="31" t="s">
+      <c r="E61" s="31" t="s">
         <v>772</v>
       </c>
-      <c r="G60" s="31" t="s">
+      <c r="G61" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="I60" s="31">
+      <c r="I61" s="31">
         <v>1.55</v>
       </c>
-      <c r="J60" s="3"/>
-      <c r="K60" s="3">
+      <c r="J61" s="3"/>
+      <c r="K61" s="3">
         <v>0.1</v>
       </c>
-      <c r="L60" s="3">
+      <c r="L61" s="3">
         <v>3</v>
       </c>
-      <c r="M60" s="3">
+      <c r="M61" s="3">
         <v>1</v>
       </c>
-      <c r="N60" s="31">
-        <f>(K60+L60)/6</f>
+      <c r="N61" s="31">
+        <f>(K61+L61)/6</f>
         <v>0.51666666666666672</v>
       </c>
-      <c r="O60" s="3"/>
-      <c r="Q60" s="39"/>
-      <c r="R60" s="2" t="s">
+      <c r="O61" s="3"/>
+      <c r="Q61" s="39"/>
+      <c r="R61" s="2" t="s">
         <v>874</v>
       </c>
     </row>
-    <row r="61" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="37" t="b">
+    <row r="62" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B61" s="37" t="s">
+      <c r="B62" s="37" t="s">
         <v>775</v>
       </c>
-      <c r="C61" s="37" t="s">
+      <c r="C62" s="37" t="s">
         <v>755</v>
       </c>
-      <c r="D61" s="37" t="s">
+      <c r="D62" s="37" t="s">
         <v>740</v>
       </c>
-      <c r="E61" s="37" t="s">
+      <c r="E62" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="H61" s="38"/>
-      <c r="I61" s="38"/>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B62" s="31" t="s">
+      <c r="H62" s="38"/>
+      <c r="I62" s="38"/>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B63" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D62" s="31" t="s">
+      <c r="D63" s="31" t="s">
         <v>774</v>
       </c>
-      <c r="E62" s="31" t="s">
+      <c r="E63" s="31" t="s">
         <v>773</v>
       </c>
-      <c r="G62" s="31" t="s">
+      <c r="G63" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="I62" s="31">
+      <c r="I63" s="31">
         <v>1.55</v>
       </c>
-      <c r="J62" s="3"/>
-      <c r="K62" s="3">
+      <c r="J63" s="3"/>
+      <c r="K63" s="3">
         <v>0.1</v>
       </c>
-      <c r="L62" s="3">
+      <c r="L63" s="3">
         <v>3</v>
       </c>
-      <c r="M62" s="3">
+      <c r="M63" s="3">
         <v>1</v>
       </c>
-      <c r="N62" s="31">
-        <f>(K62+L62)/6</f>
+      <c r="N63" s="31">
+        <f>(K63+L63)/6</f>
         <v>0.51666666666666672</v>
       </c>
-      <c r="O62" s="3"/>
-      <c r="Q62" s="39"/>
-      <c r="R62" s="2" t="s">
+      <c r="O63" s="3"/>
+      <c r="Q63" s="39"/>
+      <c r="R63" s="2" t="s">
         <v>874</v>
       </c>
     </row>
-    <row r="63" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="37" t="b">
+    <row r="64" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B63" s="37" t="s">
+      <c r="B64" s="37" t="s">
         <v>776</v>
       </c>
-      <c r="C63" s="37" t="s">
+      <c r="C64" s="37" t="s">
         <v>756</v>
       </c>
-      <c r="D63" s="37" t="s">
+      <c r="D64" s="37" t="s">
         <v>741</v>
       </c>
-      <c r="E63" s="37" t="s">
+      <c r="E64" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="H63" s="38"/>
-      <c r="I63" s="38"/>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B64" s="31" t="s">
+      <c r="H64" s="38"/>
+      <c r="I64" s="38"/>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B65" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D64" s="31" t="s">
+      <c r="D65" s="31" t="s">
         <v>778</v>
       </c>
-      <c r="E64" s="31" t="s">
+      <c r="E65" s="31" t="s">
         <v>777</v>
       </c>
-      <c r="G64" s="31" t="s">
+      <c r="G65" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="I64" s="31">
+      <c r="I65" s="31">
         <v>1.55</v>
       </c>
-      <c r="J64" s="3"/>
-      <c r="K64" s="3">
+      <c r="J65" s="3"/>
+      <c r="K65" s="3">
         <v>0.1</v>
       </c>
-      <c r="L64" s="3">
+      <c r="L65" s="3">
         <v>3</v>
       </c>
-      <c r="M64" s="3">
+      <c r="M65" s="3">
         <v>1</v>
       </c>
-      <c r="N64" s="31">
-        <f>(K64+L64)/6</f>
+      <c r="N65" s="31">
+        <f>(K65+L65)/6</f>
         <v>0.51666666666666672</v>
       </c>
-      <c r="O64" s="3"/>
-      <c r="Q64" s="39"/>
-      <c r="R64" s="2" t="s">
+      <c r="O65" s="3"/>
+      <c r="Q65" s="39"/>
+      <c r="R65" s="2" t="s">
         <v>874</v>
       </c>
     </row>
-    <row r="65" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="37" t="b">
+    <row r="66" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B65" s="37" t="s">
+      <c r="B66" s="37" t="s">
         <v>797</v>
       </c>
-      <c r="C65" s="37" t="s">
+      <c r="C66" s="37" t="s">
         <v>798</v>
       </c>
-      <c r="D65" s="37" t="s">
+      <c r="D66" s="37" t="s">
         <v>796</v>
       </c>
-      <c r="E65" s="37" t="s">
+      <c r="E66" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="H65" s="38"/>
-      <c r="I65" s="38"/>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B66" s="31" t="s">
+      <c r="H66" s="38"/>
+      <c r="I66" s="38"/>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B67" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D66" s="31" t="s">
+      <c r="D67" s="31" t="s">
         <v>800</v>
       </c>
-      <c r="E66" s="31" t="s">
+      <c r="E67" s="31" t="s">
         <v>799</v>
       </c>
-      <c r="G66" s="31" t="s">
+      <c r="G67" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="I66" s="31">
+      <c r="I67" s="31">
         <v>1.55</v>
       </c>
-      <c r="J66" s="3"/>
-      <c r="K66" s="3">
+      <c r="J67" s="3"/>
+      <c r="K67" s="3">
         <v>0.1</v>
       </c>
-      <c r="L66" s="3">
+      <c r="L67" s="3">
         <v>3</v>
       </c>
-      <c r="M66" s="3">
+      <c r="M67" s="3">
         <v>1</v>
       </c>
-      <c r="N66" s="31">
-        <f>(K66+L66)/6</f>
+      <c r="N67" s="31">
+        <f>(K67+L67)/6</f>
         <v>0.51666666666666672</v>
       </c>
-      <c r="O66" s="3"/>
-      <c r="Q66" s="39"/>
-      <c r="R66" s="2" t="s">
+      <c r="O67" s="3"/>
+      <c r="Q67" s="39"/>
+      <c r="R67" s="2" t="s">
         <v>874</v>
       </c>
     </row>
-    <row r="67" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="37" t="b">
+    <row r="68" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B67" s="37" t="s">
+      <c r="B68" s="37" t="s">
         <v>791</v>
       </c>
-      <c r="C67" s="37" t="s">
+      <c r="C68" s="37" t="s">
         <v>793</v>
       </c>
-      <c r="D67" s="37" t="s">
+      <c r="D68" s="37" t="s">
         <v>792</v>
       </c>
-      <c r="E67" s="37" t="s">
+      <c r="E68" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="H67" s="38"/>
-      <c r="I67" s="38"/>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B68" s="31" t="s">
+      <c r="H68" s="38"/>
+      <c r="I68" s="38"/>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B69" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D68" s="31" t="s">
+      <c r="D69" s="31" t="s">
         <v>795</v>
       </c>
-      <c r="E68" s="31" t="s">
+      <c r="E69" s="31" t="s">
         <v>794</v>
       </c>
-      <c r="G68" s="31" t="s">
+      <c r="G69" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="I68" s="31">
+      <c r="I69" s="31">
         <v>1.55</v>
       </c>
-      <c r="J68" s="3"/>
-      <c r="K68" s="3">
+      <c r="J69" s="3"/>
+      <c r="K69" s="3">
         <v>0.1</v>
       </c>
-      <c r="L68" s="3">
+      <c r="L69" s="3">
         <v>3</v>
       </c>
-      <c r="M68" s="3">
+      <c r="M69" s="3">
         <v>1</v>
       </c>
-      <c r="N68" s="31">
-        <f>(K68+L68)/6</f>
+      <c r="N69" s="31">
+        <f>(K69+L69)/6</f>
         <v>0.51666666666666672</v>
       </c>
-      <c r="O68" s="3"/>
-      <c r="Q68" s="39"/>
-      <c r="R68" s="2" t="s">
+      <c r="O69" s="3"/>
+      <c r="Q69" s="39"/>
+      <c r="R69" s="2" t="s">
         <v>874</v>
       </c>
     </row>
-    <row r="69" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="37" t="b">
+    <row r="70" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="B69" s="37" t="s">
+      <c r="B70" s="37" t="s">
         <v>784</v>
       </c>
-      <c r="C69" s="37" t="s">
+      <c r="C70" s="37" t="s">
         <v>786</v>
       </c>
-      <c r="D69" s="37" t="s">
+      <c r="D70" s="37" t="s">
         <v>785</v>
       </c>
-      <c r="E69" s="37" t="s">
+      <c r="E70" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="H69" s="38"/>
-      <c r="I69" s="38"/>
-    </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B70" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D70" s="31" t="s">
-        <v>789</v>
-      </c>
-      <c r="E70" s="31" t="s">
-        <v>787</v>
-      </c>
-      <c r="G70" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="I70" s="31">
-        <v>1</v>
-      </c>
-      <c r="J70" s="3"/>
-      <c r="K70" s="3"/>
-      <c r="L70" s="3"/>
-      <c r="M70" s="3"/>
-      <c r="N70" s="3"/>
-      <c r="O70" s="3"/>
-      <c r="Q70" s="39"/>
-      <c r="R70" s="2"/>
+      <c r="H70" s="38"/>
+      <c r="I70" s="38"/>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B71" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D71" s="31" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E71" s="31" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="G71" s="31" t="s">
         <v>619</v>
@@ -9236,37 +9238,43 @@
       <c r="Q71" s="39"/>
       <c r="R71" s="2"/>
     </row>
-    <row r="72" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="37" t="b">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B72" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D72" s="31" t="s">
+        <v>790</v>
+      </c>
+      <c r="E72" s="31" t="s">
+        <v>788</v>
+      </c>
+      <c r="G72" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="I72" s="31">
         <v>1</v>
       </c>
-      <c r="B72" s="37" t="s">
-        <v>821</v>
-      </c>
-      <c r="C72" s="37" t="s">
-        <v>829</v>
-      </c>
-      <c r="D72" s="37" t="s">
-        <v>813</v>
-      </c>
-      <c r="E72" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="H72" s="38"/>
-      <c r="I72" s="38"/>
+      <c r="J72" s="3"/>
+      <c r="K72" s="3"/>
+      <c r="L72" s="3"/>
+      <c r="M72" s="3"/>
+      <c r="N72" s="3"/>
+      <c r="O72" s="3"/>
+      <c r="Q72" s="39"/>
+      <c r="R72" s="2"/>
     </row>
     <row r="73" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="37" t="b">
         <v>1</v>
       </c>
       <c r="B73" s="37" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="C73" s="37" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D73" s="37" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E73" s="37" t="s">
         <v>68</v>
@@ -9279,13 +9287,13 @@
         <v>1</v>
       </c>
       <c r="B74" s="37" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="C74" s="37" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="D74" s="37" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="E74" s="37" t="s">
         <v>68</v>
@@ -9298,13 +9306,13 @@
         <v>1</v>
       </c>
       <c r="B75" s="37" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="C75" s="37" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="D75" s="37" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E75" s="37" t="s">
         <v>68</v>
@@ -9317,13 +9325,13 @@
         <v>1</v>
       </c>
       <c r="B76" s="37" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C76" s="37" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="D76" s="37" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="E76" s="37" t="s">
         <v>68</v>
@@ -9336,13 +9344,13 @@
         <v>1</v>
       </c>
       <c r="B77" s="37" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="C77" s="37" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="D77" s="37" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E77" s="37" t="s">
         <v>68</v>
@@ -9355,13 +9363,13 @@
         <v>1</v>
       </c>
       <c r="B78" s="37" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C78" s="37" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="D78" s="37" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E78" s="37" t="s">
         <v>68</v>
@@ -9374,13 +9382,13 @@
         <v>1</v>
       </c>
       <c r="B79" s="37" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="C79" s="37" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="D79" s="37" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E79" s="37" t="s">
         <v>68</v>
@@ -9393,13 +9401,13 @@
         <v>1</v>
       </c>
       <c r="B80" s="37" t="s">
-        <v>809</v>
+        <v>828</v>
       </c>
       <c r="C80" s="37" t="s">
-        <v>810</v>
+        <v>836</v>
       </c>
       <c r="D80" s="37" t="s">
-        <v>811</v>
+        <v>820</v>
       </c>
       <c r="E80" s="37" t="s">
         <v>68</v>
@@ -9412,13 +9420,13 @@
         <v>1</v>
       </c>
       <c r="B81" s="37" t="s">
-        <v>899</v>
+        <v>809</v>
       </c>
       <c r="C81" s="37" t="s">
-        <v>898</v>
+        <v>810</v>
       </c>
       <c r="D81" s="37" t="s">
-        <v>897</v>
+        <v>811</v>
       </c>
       <c r="E81" s="37" t="s">
         <v>68</v>
@@ -9426,72 +9434,54 @@
       <c r="H81" s="38"/>
       <c r="I81" s="38"/>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B82" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D82" s="46" t="s">
-        <v>902</v>
-      </c>
-      <c r="E82" s="46" t="s">
-        <v>900</v>
-      </c>
-      <c r="G82" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="I82" s="4">
-        <v>8</v>
-      </c>
-      <c r="J82" s="31"/>
-      <c r="K82" s="31">
-        <v>7</v>
-      </c>
-      <c r="L82" s="31">
-        <v>10</v>
-      </c>
-      <c r="M82" s="31">
-        <v>8</v>
-      </c>
-      <c r="N82" s="31">
-        <f>(K82+L82)/6</f>
-        <v>2.8333333333333335</v>
-      </c>
-      <c r="O82" s="31">
-        <v>0.5</v>
-      </c>
-      <c r="R82" s="31" t="s">
-        <v>874</v>
-      </c>
+    <row r="82" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B82" s="37" t="s">
+        <v>899</v>
+      </c>
+      <c r="C82" s="37" t="s">
+        <v>898</v>
+      </c>
+      <c r="D82" s="37" t="s">
+        <v>897</v>
+      </c>
+      <c r="E82" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="H82" s="38"/>
+      <c r="I82" s="38"/>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B83" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D83" s="46" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="E83" s="46" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="G83" s="31" t="s">
         <v>619</v>
       </c>
       <c r="I83" s="4">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="J83" s="31"/>
       <c r="K83" s="31">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="L83" s="31">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="M83" s="31">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="N83" s="31">
         <f>(K83+L83)/6</f>
-        <v>6</v>
+        <v>2.8333333333333335</v>
       </c>
       <c r="O83" s="31">
         <v>0.5</v>
@@ -9502,33 +9492,33 @@
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B84" s="31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D84" s="46" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="E84" s="46" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="G84" s="31" t="s">
         <v>619</v>
       </c>
       <c r="I84" s="4">
-        <v>3.8906915646632803E-2</v>
+        <v>17</v>
       </c>
       <c r="J84" s="31"/>
       <c r="K84" s="31">
-        <v>-2</v>
+        <v>16</v>
       </c>
       <c r="L84" s="31">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="M84" s="31">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="N84" s="31">
-        <f t="shared" ref="N84:N85" si="0">(K84+L84)/6</f>
-        <v>0</v>
+        <f>(K84+L84)/6</f>
+        <v>6</v>
       </c>
       <c r="O84" s="31">
         <v>0.5</v>
@@ -9542,16 +9532,16 @@
         <v>22</v>
       </c>
       <c r="D85" s="46" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="E85" s="46" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="G85" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="I85" s="53">
-        <v>1.6126334175777899E-22</v>
+      <c r="I85" s="4">
+        <v>3.8906915646632803E-2</v>
       </c>
       <c r="J85" s="31"/>
       <c r="K85" s="31">
@@ -9564,7 +9554,7 @@
         <v>0</v>
       </c>
       <c r="N85" s="31">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="N85:N86" si="0">(K85+L85)/6</f>
         <v>0</v>
       </c>
       <c r="O85" s="31">
@@ -9574,28 +9564,61 @@
         <v>874</v>
       </c>
     </row>
-    <row r="86" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="37" t="b">
-        <v>0</v>
-      </c>
-      <c r="B86" s="37" t="s">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B86" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D86" s="46" t="s">
+        <v>907</v>
+      </c>
+      <c r="E86" s="46" t="s">
+        <v>906</v>
+      </c>
+      <c r="G86" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="I86" s="53">
+        <v>1.6126334175777899E-22</v>
+      </c>
+      <c r="J86" s="31"/>
+      <c r="K86" s="31">
+        <v>-2</v>
+      </c>
+      <c r="L86" s="31">
+        <v>2</v>
+      </c>
+      <c r="M86" s="31">
+        <v>0</v>
+      </c>
+      <c r="N86" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O86" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="R86" s="31" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B87" s="37" t="s">
         <v>846</v>
       </c>
-      <c r="C86" s="37" t="s">
+      <c r="C87" s="37" t="s">
         <v>845</v>
       </c>
-      <c r="D86" s="37" t="s">
+      <c r="D87" s="37" t="s">
         <v>847</v>
       </c>
-      <c r="E86" s="37" t="s">
+      <c r="E87" s="37" t="s">
         <v>233</v>
       </c>
-      <c r="H86" s="38"/>
-      <c r="I86" s="38"/>
-    </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="I87" s="31"/>
-      <c r="J87" s="31"/>
+      <c r="H87" s="38"/>
+      <c r="I87" s="38"/>
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I88" s="31"/>
@@ -9809,8 +9832,12 @@
       <c r="I140" s="31"/>
       <c r="J140" s="31"/>
     </row>
+    <row r="141" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I141" s="31"/>
+      <c r="J141" s="31"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:AA64"/>
+  <autoFilter ref="A2:AA65"/>
   <mergeCells count="1">
     <mergeCell ref="U1:Z1"/>
   </mergeCells>

</xml_diff>

<commit_message>
Added ee and tariff to workflow
May need to change ee to act as "ee" vs "indemand" to test it with the
current analytic record? I have not tested this in the workflow,
although I have tested the economizer measure on its own.
</commit_message>
<xml_diff>
--- a/projects/dfg_test_m0_office_blend.xlsx
+++ b/projects/dfg_test_m0_office_blend.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2541" uniqueCount="919">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2540" uniqueCount="919">
   <si>
     <t>type</t>
   </si>
@@ -2227,12 +2227,6 @@
     <t>Depth of perimeter thermal zone</t>
   </si>
   <si>
-    <t>floor_to_floor_height</t>
-  </si>
-  <si>
-    <t>Floor to floor height</t>
-  </si>
-  <si>
     <t>aspect_ratio_ns_to_ew</t>
   </si>
   <si>
@@ -2798,6 +2792,12 @@
   </si>
   <si>
     <t>area D</t>
+  </si>
+  <si>
+    <t>Floor to Floor Height Multiplier</t>
+  </si>
+  <si>
+    <t>floor_to_floor_multiplier</t>
   </si>
 </sst>
 </file>
@@ -4777,7 +4777,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -4881,7 +4881,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7022,8 +7021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7059,7 +7058,7 @@
         <v>436</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>437</v>
@@ -7070,7 +7069,7 @@
         <v>456</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>457</v>
@@ -7081,7 +7080,7 @@
         <v>469</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>614</v>
@@ -7163,7 +7162,7 @@
         <v>39</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>471</v>
@@ -7174,7 +7173,7 @@
         <v>25</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>660</v>
@@ -7253,7 +7252,7 @@
         <v>451</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -7355,7 +7354,7 @@
         <v>29</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -7386,7 +7385,7 @@
         <v>648</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -7409,10 +7408,10 @@
         <v>649</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -7420,10 +7419,10 @@
         <v>649</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="C44" s="31" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="D44" s="2"/>
     </row>
@@ -7454,8 +7453,8 @@
   <dimension ref="A1:Z141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D36" sqref="D36:I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7510,14 +7509,14 @@
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
       <c r="T1" s="5"/>
-      <c r="U1" s="54" t="s">
+      <c r="U1" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54"/>
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="53"/>
+      <c r="Y1" s="53"/>
+      <c r="Z1" s="53"/>
     </row>
     <row r="2" spans="1:26" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -7553,7 +7552,7 @@
         <v>36</v>
       </c>
       <c r="F3" s="50" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="G3" s="15" t="s">
         <v>11</v>
@@ -7618,13 +7617,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>68</v>
@@ -7637,16 +7636,16 @@
         <v>21</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="G5" s="31" t="s">
         <v>618</v>
       </c>
       <c r="I5" s="31" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="J5" s="31"/>
     </row>
@@ -7655,16 +7654,16 @@
         <v>21</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="G6" s="31" t="s">
         <v>618</v>
       </c>
       <c r="I6" s="31" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="J6" s="31"/>
     </row>
@@ -7673,16 +7672,16 @@
         <v>21</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="G7" s="31" t="s">
         <v>618</v>
       </c>
       <c r="I7" s="52" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="J7" s="31"/>
     </row>
@@ -7691,16 +7690,16 @@
         <v>21</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="G8" s="31" t="s">
         <v>618</v>
       </c>
       <c r="I8" s="52" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="J8" s="31"/>
     </row>
@@ -7709,13 +7708,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="E9" s="37" t="s">
         <v>233</v>
@@ -7773,7 +7772,7 @@
         <v>104</v>
       </c>
       <c r="I12" s="31" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
     </row>
     <row r="13" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -7781,7 +7780,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="C13" s="37" t="s">
         <v>717</v>
@@ -7810,7 +7809,7 @@
         <v>618</v>
       </c>
       <c r="I14" s="31" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -7826,13 +7825,13 @@
         <v>21</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="E15" s="31" t="s">
         <v>719</v>
       </c>
       <c r="F15" s="31" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="G15" s="31" t="s">
         <v>619</v>
@@ -7857,7 +7856,7 @@
       <c r="P15" s="4"/>
       <c r="Q15" s="3"/>
       <c r="R15" s="31" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
@@ -7865,7 +7864,7 @@
         <v>21</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="E16" s="31" t="s">
         <v>720</v>
@@ -7884,17 +7883,17 @@
         <v>21</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="F17" s="30"/>
       <c r="G17" s="30" t="s">
         <v>104</v>
       </c>
       <c r="I17" s="31" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="J17" s="31"/>
     </row>
@@ -7903,7 +7902,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="C18" s="37" t="s">
         <v>717</v>
@@ -7932,7 +7931,7 @@
         <v>618</v>
       </c>
       <c r="I19" s="31" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -7948,13 +7947,13 @@
         <v>21</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="E20" s="31" t="s">
         <v>719</v>
       </c>
       <c r="F20" s="31" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="G20" s="31" t="s">
         <v>619</v>
@@ -7979,7 +7978,7 @@
       <c r="P20" s="4"/>
       <c r="Q20" s="3"/>
       <c r="R20" s="31" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -7987,7 +7986,7 @@
         <v>21</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="E21" s="31" t="s">
         <v>720</v>
@@ -8006,17 +8005,17 @@
         <v>21</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="E22" s="31" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="F22" s="30"/>
       <c r="G22" s="30" t="s">
         <v>104</v>
       </c>
       <c r="I22" s="31" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="J22" s="31"/>
     </row>
@@ -8025,7 +8024,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="37" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="C23" s="37" t="s">
         <v>717</v>
@@ -8054,7 +8053,7 @@
         <v>618</v>
       </c>
       <c r="I24" s="31" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -8070,13 +8069,13 @@
         <v>21</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="E25" s="31" t="s">
         <v>719</v>
       </c>
       <c r="F25" s="31" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="G25" s="31" t="s">
         <v>619</v>
@@ -8101,7 +8100,7 @@
       <c r="P25" s="4"/>
       <c r="Q25" s="3"/>
       <c r="R25" s="31" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -8109,7 +8108,7 @@
         <v>21</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="E26" s="31" t="s">
         <v>720</v>
@@ -8128,17 +8127,17 @@
         <v>21</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="E27" s="31" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="F27" s="30"/>
       <c r="G27" s="30" t="s">
         <v>104</v>
       </c>
       <c r="I27" s="31" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="J27" s="31"/>
     </row>
@@ -8147,7 +8146,7 @@
         <v>1</v>
       </c>
       <c r="B28" s="37" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="C28" s="37" t="s">
         <v>717</v>
@@ -8176,7 +8175,7 @@
         <v>618</v>
       </c>
       <c r="I29" s="31" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
@@ -8192,13 +8191,13 @@
         <v>21</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="E30" s="31" t="s">
         <v>719</v>
       </c>
       <c r="F30" s="31" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="G30" s="31" t="s">
         <v>619</v>
@@ -8223,7 +8222,7 @@
       <c r="P30" s="4"/>
       <c r="Q30" s="3"/>
       <c r="R30" s="31" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
@@ -8231,7 +8230,7 @@
         <v>21</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="E31" s="31" t="s">
         <v>720</v>
@@ -8250,17 +8249,17 @@
         <v>21</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="E32" s="31" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="F32" s="30"/>
       <c r="G32" s="30" t="s">
         <v>104</v>
       </c>
       <c r="I32" s="31" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="J32" s="31"/>
     </row>
@@ -8288,7 +8287,7 @@
         <v>21</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="E34" s="31" t="s">
         <v>725</v>
@@ -8339,19 +8338,16 @@
         <v>21</v>
       </c>
       <c r="D36" s="31" t="s">
-        <v>729</v>
+        <v>917</v>
       </c>
       <c r="E36" s="31" t="s">
-        <v>728</v>
+        <v>918</v>
       </c>
       <c r="G36" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="H36" s="31" t="s">
-        <v>658</v>
-      </c>
       <c r="I36" s="4">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J36" s="31"/>
     </row>
@@ -8360,10 +8356,10 @@
         <v>21</v>
       </c>
       <c r="D37" s="31" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="E37" s="31" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="G37" s="31" t="s">
         <v>619</v>
@@ -8378,16 +8374,16 @@
         <v>21</v>
       </c>
       <c r="D38" s="31" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="E38" s="31" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="G38" s="31" t="s">
         <v>618</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="J38" s="31"/>
     </row>
@@ -8396,13 +8392,13 @@
         <v>1</v>
       </c>
       <c r="B39" s="37" t="s">
+        <v>835</v>
+      </c>
+      <c r="C39" s="37" t="s">
+        <v>836</v>
+      </c>
+      <c r="D39" s="37" t="s">
         <v>837</v>
-      </c>
-      <c r="C39" s="37" t="s">
-        <v>838</v>
-      </c>
-      <c r="D39" s="37" t="s">
-        <v>839</v>
       </c>
       <c r="E39" s="37" t="s">
         <v>68</v>
@@ -8415,10 +8411,10 @@
         <v>21</v>
       </c>
       <c r="D40" s="46" t="s">
+        <v>757</v>
+      </c>
+      <c r="E40" s="46" t="s">
         <v>759</v>
-      </c>
-      <c r="E40" s="46" t="s">
-        <v>761</v>
       </c>
       <c r="G40" s="31" t="s">
         <v>619</v>
@@ -8444,7 +8440,7 @@
         <v>0.5</v>
       </c>
       <c r="R40" s="31" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
@@ -8452,10 +8448,10 @@
         <v>21</v>
       </c>
       <c r="D41" s="46" t="s">
+        <v>758</v>
+      </c>
+      <c r="E41" s="46" t="s">
         <v>760</v>
-      </c>
-      <c r="E41" s="46" t="s">
-        <v>762</v>
       </c>
       <c r="G41" s="31" t="s">
         <v>619</v>
@@ -8481,7 +8477,7 @@
         <v>0.5</v>
       </c>
       <c r="R41" s="31" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="42" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -8489,13 +8485,13 @@
         <v>1</v>
       </c>
       <c r="B42" s="37" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="C42" s="37" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="D42" s="37" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="E42" s="37" t="s">
         <v>68</v>
@@ -8508,16 +8504,16 @@
         <v>22</v>
       </c>
       <c r="D43" s="31" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="E43" s="31" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="G43" s="31" t="s">
         <v>619</v>
       </c>
       <c r="I43" s="31">
-        <v>1.55</v>
+        <v>1</v>
       </c>
       <c r="J43" s="3"/>
       <c r="K43" s="3">
@@ -8536,7 +8532,7 @@
       <c r="O43" s="3"/>
       <c r="Q43" s="39"/>
       <c r="R43" s="2" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="44" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -8544,13 +8540,13 @@
         <v>1</v>
       </c>
       <c r="B44" s="37" t="s">
+        <v>746</v>
+      </c>
+      <c r="C44" s="37" t="s">
         <v>748</v>
       </c>
-      <c r="C44" s="37" t="s">
-        <v>750</v>
-      </c>
       <c r="D44" s="37" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="E44" s="37" t="s">
         <v>68</v>
@@ -8563,16 +8559,16 @@
         <v>22</v>
       </c>
       <c r="D45" s="31" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="E45" s="31" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="G45" s="31" t="s">
         <v>619</v>
       </c>
       <c r="I45" s="31">
-        <v>1.55</v>
+        <v>1</v>
       </c>
       <c r="J45" s="3"/>
       <c r="K45" s="3">
@@ -8591,7 +8587,7 @@
       <c r="O45" s="3"/>
       <c r="Q45" s="39"/>
       <c r="R45" s="2" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="46" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -8599,13 +8595,13 @@
         <v>1</v>
       </c>
       <c r="B46" s="37" t="s">
+        <v>745</v>
+      </c>
+      <c r="C46" s="37" t="s">
         <v>747</v>
       </c>
-      <c r="C46" s="37" t="s">
-        <v>749</v>
-      </c>
       <c r="D46" s="37" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="E46" s="37" t="s">
         <v>68</v>
@@ -8618,16 +8614,16 @@
         <v>22</v>
       </c>
       <c r="D47" s="31" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="E47" s="31" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="G47" s="31" t="s">
         <v>619</v>
       </c>
       <c r="I47" s="31">
-        <v>1.55</v>
+        <v>1</v>
       </c>
       <c r="J47" s="3"/>
       <c r="K47" s="3">
@@ -8646,7 +8642,7 @@
       <c r="O47" s="3"/>
       <c r="Q47" s="39"/>
       <c r="R47" s="2" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="48" spans="1:18" s="47" customFormat="1" x14ac:dyDescent="0.25">
@@ -8654,13 +8650,13 @@
         <v>1</v>
       </c>
       <c r="B48" s="47" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="C48" s="47" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="D48" s="47" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="E48" s="47" t="s">
         <v>68</v>
@@ -8674,13 +8670,13 @@
         <v>1</v>
       </c>
       <c r="B49" s="37" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="C49" s="37" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="D49" s="37" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="E49" s="37" t="s">
         <v>68</v>
@@ -8693,13 +8689,13 @@
         <v>1</v>
       </c>
       <c r="B50" s="37" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="C50" s="37" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="D50" s="37" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="E50" s="37" t="s">
         <v>68</v>
@@ -8740,7 +8736,7 @@
         <v>619</v>
       </c>
       <c r="H52" s="31" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="I52" s="31">
         <v>0</v>
@@ -8759,13 +8755,13 @@
         <v>1</v>
       </c>
       <c r="B53" s="47" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="C53" s="47" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="D53" s="47" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="E53" s="47" t="s">
         <v>68</v>
@@ -8779,10 +8775,10 @@
         <v>21</v>
       </c>
       <c r="D54" s="31" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="E54" s="31" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="G54" s="31" t="s">
         <v>619</v>
@@ -8804,10 +8800,10 @@
         <v>21</v>
       </c>
       <c r="D55" s="31" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="E55" s="31" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="G55" s="31" t="s">
         <v>619</v>
@@ -8829,10 +8825,10 @@
         <v>21</v>
       </c>
       <c r="D56" s="31" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="E56" s="31" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="G56" s="31" t="s">
         <v>619</v>
@@ -8854,10 +8850,10 @@
         <v>21</v>
       </c>
       <c r="D57" s="31" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="E57" s="31" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="G57" s="31" t="s">
         <v>619</v>
@@ -8879,13 +8875,13 @@
         <v>1</v>
       </c>
       <c r="B58" s="37" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="C58" s="37" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="D58" s="37" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="E58" s="37" t="s">
         <v>68</v>
@@ -8898,10 +8894,10 @@
         <v>21</v>
       </c>
       <c r="D59" s="31" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="E59" s="31" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="G59" s="31" t="s">
         <v>619</v>
@@ -8923,13 +8919,13 @@
         <v>1</v>
       </c>
       <c r="B60" s="37" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="C60" s="37" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="D60" s="37" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E60" s="37" t="s">
         <v>68</v>
@@ -8942,16 +8938,16 @@
         <v>22</v>
       </c>
       <c r="D61" s="31" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="E61" s="31" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="G61" s="31" t="s">
         <v>619</v>
       </c>
       <c r="I61" s="31">
-        <v>1.55</v>
+        <v>1</v>
       </c>
       <c r="J61" s="3"/>
       <c r="K61" s="3">
@@ -8970,7 +8966,7 @@
       <c r="O61" s="3"/>
       <c r="Q61" s="39"/>
       <c r="R61" s="2" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="62" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -8978,13 +8974,13 @@
         <v>1</v>
       </c>
       <c r="B62" s="37" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="C62" s="37" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="D62" s="37" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="E62" s="37" t="s">
         <v>68</v>
@@ -8997,16 +8993,16 @@
         <v>22</v>
       </c>
       <c r="D63" s="31" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="E63" s="31" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="G63" s="31" t="s">
         <v>619</v>
       </c>
       <c r="I63" s="31">
-        <v>1.55</v>
+        <v>1</v>
       </c>
       <c r="J63" s="3"/>
       <c r="K63" s="3">
@@ -9025,7 +9021,7 @@
       <c r="O63" s="3"/>
       <c r="Q63" s="39"/>
       <c r="R63" s="2" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="64" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -9033,13 +9029,13 @@
         <v>1</v>
       </c>
       <c r="B64" s="37" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="C64" s="37" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="D64" s="37" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="E64" s="37" t="s">
         <v>68</v>
@@ -9052,16 +9048,16 @@
         <v>22</v>
       </c>
       <c r="D65" s="31" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="E65" s="31" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="G65" s="31" t="s">
         <v>619</v>
       </c>
       <c r="I65" s="31">
-        <v>1.55</v>
+        <v>1</v>
       </c>
       <c r="J65" s="3"/>
       <c r="K65" s="3">
@@ -9080,7 +9076,7 @@
       <c r="O65" s="3"/>
       <c r="Q65" s="39"/>
       <c r="R65" s="2" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="66" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -9088,13 +9084,13 @@
         <v>1</v>
       </c>
       <c r="B66" s="37" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C66" s="37" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="D66" s="37" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="E66" s="37" t="s">
         <v>68</v>
@@ -9107,16 +9103,16 @@
         <v>22</v>
       </c>
       <c r="D67" s="31" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="E67" s="31" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="G67" s="31" t="s">
         <v>619</v>
       </c>
       <c r="I67" s="31">
-        <v>1.55</v>
+        <v>1</v>
       </c>
       <c r="J67" s="3"/>
       <c r="K67" s="3">
@@ -9135,7 +9131,7 @@
       <c r="O67" s="3"/>
       <c r="Q67" s="39"/>
       <c r="R67" s="2" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="68" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -9143,13 +9139,13 @@
         <v>1</v>
       </c>
       <c r="B68" s="37" t="s">
+        <v>788</v>
+      </c>
+      <c r="C68" s="37" t="s">
         <v>790</v>
       </c>
-      <c r="C68" s="37" t="s">
-        <v>792</v>
-      </c>
       <c r="D68" s="37" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="E68" s="37" t="s">
         <v>68</v>
@@ -9162,16 +9158,16 @@
         <v>22</v>
       </c>
       <c r="D69" s="31" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="E69" s="31" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="G69" s="31" t="s">
         <v>619</v>
       </c>
       <c r="I69" s="31">
-        <v>1.55</v>
+        <v>1</v>
       </c>
       <c r="J69" s="3"/>
       <c r="K69" s="3">
@@ -9190,7 +9186,7 @@
       <c r="O69" s="3"/>
       <c r="Q69" s="39"/>
       <c r="R69" s="2" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="70" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -9198,13 +9194,13 @@
         <v>1</v>
       </c>
       <c r="B70" s="37" t="s">
+        <v>781</v>
+      </c>
+      <c r="C70" s="37" t="s">
         <v>783</v>
       </c>
-      <c r="C70" s="37" t="s">
-        <v>785</v>
-      </c>
       <c r="D70" s="37" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="E70" s="37" t="s">
         <v>68</v>
@@ -9217,10 +9213,10 @@
         <v>21</v>
       </c>
       <c r="D71" s="31" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="E71" s="31" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="G71" s="31" t="s">
         <v>619</v>
@@ -9242,10 +9238,10 @@
         <v>21</v>
       </c>
       <c r="D72" s="31" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="E72" s="31" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="G72" s="31" t="s">
         <v>619</v>
@@ -9267,13 +9263,13 @@
         <v>1</v>
       </c>
       <c r="B73" s="37" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="C73" s="37" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="D73" s="37" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="E73" s="37" t="s">
         <v>68</v>
@@ -9286,13 +9282,13 @@
         <v>1</v>
       </c>
       <c r="B74" s="37" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="C74" s="37" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="D74" s="37" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="E74" s="37" t="s">
         <v>68</v>
@@ -9305,13 +9301,13 @@
         <v>1</v>
       </c>
       <c r="B75" s="37" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="C75" s="37" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="D75" s="37" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="E75" s="37" t="s">
         <v>68</v>
@@ -9324,13 +9320,13 @@
         <v>1</v>
       </c>
       <c r="B76" s="37" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C76" s="37" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="D76" s="37" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="E76" s="37" t="s">
         <v>68</v>
@@ -9343,13 +9339,13 @@
         <v>1</v>
       </c>
       <c r="B77" s="37" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="C77" s="37" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="D77" s="37" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="E77" s="37" t="s">
         <v>68</v>
@@ -9362,13 +9358,13 @@
         <v>1</v>
       </c>
       <c r="B78" s="37" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="C78" s="37" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="D78" s="37" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="E78" s="37" t="s">
         <v>68</v>
@@ -9381,13 +9377,13 @@
         <v>1</v>
       </c>
       <c r="B79" s="37" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="C79" s="37" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="D79" s="37" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="E79" s="37" t="s">
         <v>68</v>
@@ -9400,13 +9396,13 @@
         <v>1</v>
       </c>
       <c r="B80" s="37" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="C80" s="37" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="D80" s="37" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="E80" s="37" t="s">
         <v>68</v>
@@ -9419,13 +9415,13 @@
         <v>1</v>
       </c>
       <c r="B81" s="37" t="s">
+        <v>806</v>
+      </c>
+      <c r="C81" s="37" t="s">
+        <v>807</v>
+      </c>
+      <c r="D81" s="37" t="s">
         <v>808</v>
-      </c>
-      <c r="C81" s="37" t="s">
-        <v>809</v>
-      </c>
-      <c r="D81" s="37" t="s">
-        <v>810</v>
       </c>
       <c r="E81" s="37" t="s">
         <v>68</v>
@@ -9438,13 +9434,13 @@
         <v>1</v>
       </c>
       <c r="B82" s="37" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="C82" s="37" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="D82" s="37" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="E82" s="37" t="s">
         <v>68</v>
@@ -9457,10 +9453,10 @@
         <v>21</v>
       </c>
       <c r="D83" s="46" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="E83" s="46" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="G83" s="31" t="s">
         <v>619</v>
@@ -9486,7 +9482,7 @@
         <v>0.5</v>
       </c>
       <c r="R83" s="31" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.25">
@@ -9494,10 +9490,10 @@
         <v>21</v>
       </c>
       <c r="D84" s="46" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="E84" s="46" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="G84" s="31" t="s">
         <v>619</v>
@@ -9523,7 +9519,7 @@
         <v>0.5</v>
       </c>
       <c r="R84" s="31" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.25">
@@ -9531,16 +9527,16 @@
         <v>22</v>
       </c>
       <c r="D85" s="46" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="E85" s="46" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="G85" s="31" t="s">
         <v>619</v>
       </c>
       <c r="I85" s="4">
-        <v>3.8906915646632803E-2</v>
+        <v>0</v>
       </c>
       <c r="J85" s="31"/>
       <c r="K85" s="31">
@@ -9560,7 +9556,7 @@
         <v>0.5</v>
       </c>
       <c r="R85" s="31" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.25">
@@ -9568,16 +9564,16 @@
         <v>22</v>
       </c>
       <c r="D86" s="46" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="E86" s="46" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="G86" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="I86" s="53">
-        <v>1.6126334175777899E-22</v>
+      <c r="I86" s="4">
+        <v>0</v>
       </c>
       <c r="J86" s="31"/>
       <c r="K86" s="31">
@@ -9597,7 +9593,7 @@
         <v>0.5</v>
       </c>
       <c r="R86" s="31" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="87" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -9605,13 +9601,13 @@
         <v>1</v>
       </c>
       <c r="B87" s="37" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="C87" s="37" t="s">
+        <v>842</v>
+      </c>
+      <c r="D87" s="37" t="s">
         <v>844</v>
-      </c>
-      <c r="D87" s="37" t="s">
-        <v>846</v>
       </c>
       <c r="E87" s="37" t="s">
         <v>233</v>
@@ -9896,7 +9892,7 @@
         <v>459</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="C2" s="44" t="s">
         <v>635</v>
@@ -9935,7 +9931,7 @@
         <v>627</v>
       </c>
       <c r="B3" s="51" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="C3" s="44" t="s">
         <v>640</v>
@@ -9974,7 +9970,7 @@
         <v>642</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="C4" s="40" t="s">
         <v>636</v>
@@ -10007,7 +10003,7 @@
         <v>643</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="C5" s="40" t="s">
         <v>637</v>
@@ -10040,7 +10036,7 @@
         <v>644</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="C6" s="40" t="s">
         <v>639</v>
@@ -10073,7 +10069,7 @@
         <v>645</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="C7" s="40" t="s">
         <v>638</v>
@@ -10813,14 +10809,14 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="40" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="C32" s="40"/>
       <c r="D32" s="40" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="E32" s="40"/>
       <c r="F32" s="40" t="s">

</xml_diff>